<commit_message>
Dash improved, sword slash init
</commit_message>
<xml_diff>
--- a/Assets/Ideas, please open when you come back.xlsx
+++ b/Assets/Ideas, please open when you come back.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Unity Projects\Travis\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4392E1-AB8E-4282-B5C6-A61B2B8324E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB8ECD8-46C9-442A-B5F8-C2140E0847B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Idea</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>Not started / Needs MoCap</t>
+  </si>
+  <si>
+    <t>Nero inspired sword power</t>
+  </si>
+  <si>
+    <t>As Travis holds a button, he will charge his sword with the equipped power (make him twirl the sword once he has the attacked charged up), making it light on fire, be covered in electricity, ice, etc. This effect will also be achieved by pressing the same button just after an attack lands</t>
+  </si>
+  <si>
+    <t>Shooting from the sword</t>
+  </si>
+  <si>
+    <t>When you shoot any power, it will come out of the sword, instead of the hand (if not fighting with the sword), Travis will twirl his sword to achieve this.</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -78,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,17 +116,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -394,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +471,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>